<commit_message>
initial checkin of XNA - probably will use WPF based, but checking this in
</commit_message>
<xml_diff>
--- a/scannertimes.xlsx
+++ b/scannertimes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>bytes at 1cm resolution</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>every 15 sec</t>
+  </si>
+  <si>
+    <t>bytes/day at 4cm</t>
   </si>
 </sst>
 </file>
@@ -374,31 +377,31 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <f>roomwidth*12*2.54</f>
-        <v>365.76</v>
+        <v>426.72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <f>roomlength*12*2.54</f>
-        <v>487.68</v>
+        <v>1645.92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -413,11 +416,11 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f>B1*B2*B3</f>
-        <v>43494676.365311995</v>
+        <v>171260288.18841603</v>
       </c>
       <c r="C4" s="2">
         <f>roomvolume/8</f>
-        <v>5436834.5456639994</v>
+        <v>21407536.023552004</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -426,7 +429,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <f>C4/4/4/4</f>
-        <v>84950.539775999991</v>
+        <v>334492.75036800007</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -444,7 +447,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f>C6*C5</f>
-        <v>489315109.10975993</v>
+        <v>1926678242.1196804</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>